<commit_message>
Added json to probability
</commit_message>
<xml_diff>
--- a/Personal_Fit_Model/nyc_popn.xlsx
+++ b/Personal_Fit_Model/nyc_popn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\realtor-insights\Personal_Fit_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01803233-7F57-4760-8AE0-3E9CEC545DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1775E38C-3CDD-4A37-B560-F2DB53EC9851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1008" windowWidth="18168" windowHeight="11952" xr2:uid="{81FBC0FE-682C-4D0A-A72B-84E50FF78C15}"/>
+    <workbookView xWindow="3072" yWindow="1008" windowWidth="18168" windowHeight="11952" xr2:uid="{81FBC0FE-682C-4D0A-A72B-84E50FF78C15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
   <si>
     <t>Total population</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>85 years and over</t>
+  </si>
+  <si>
+    <t>comm</t>
   </si>
 </sst>
 </file>
@@ -1094,9 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DB1D75-A1EB-4DBB-8EED-D9B5BD83CC4A}">
   <dimension ref="A1:K193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1105,6 +1106,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>